<commit_message>
ABD dip hourly update
</commit_message>
<xml_diff>
--- a/dip_yakalama_daily_120dip_rebound_sonuclar.xlsx
+++ b/dip_yakalama_daily_120dip_rebound_sonuclar.xlsx
@@ -14712,7 +14712,7 @@
     <row r="596">
       <c r="A596" t="inlineStr">
         <is>
-          <t>TIGO</t>
+          <t>FTAI</t>
         </is>
       </c>
       <c r="B596" t="inlineStr">
@@ -14721,16 +14721,16 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>42.05</v>
+        <v>136.06</v>
       </c>
       <c r="D596" t="n">
-        <v>62.22</v>
+        <v>276.01</v>
       </c>
       <c r="E596" t="n">
-        <v>47.97</v>
+        <v>102.86</v>
       </c>
       <c r="F596" t="n">
-        <v>1.76795</v>
+        <v>11.21528</v>
       </c>
     </row>
     <row r="597">
@@ -14856,7 +14856,7 @@
     <row r="602">
       <c r="A602" t="inlineStr">
         <is>
-          <t>AKAM</t>
+          <t>MOG-B</t>
         </is>
       </c>
       <c r="B602" t="inlineStr">
@@ -14865,22 +14865,22 @@
         </is>
       </c>
       <c r="C602" t="n">
-        <v>70.53</v>
+        <v>194.99</v>
       </c>
       <c r="D602" t="n">
-        <v>99.34999999999999</v>
+        <v>295</v>
       </c>
       <c r="E602" t="n">
-        <v>40.86</v>
+        <v>51.29</v>
       </c>
       <c r="F602" t="n">
-        <v>3.37612</v>
+        <v>6.99596</v>
       </c>
     </row>
     <row r="603">
       <c r="A603" t="inlineStr">
         <is>
-          <t>KRMN</t>
+          <t>AKAM</t>
         </is>
       </c>
       <c r="B603" t="inlineStr">
@@ -14889,22 +14889,22 @@
         </is>
       </c>
       <c r="C603" t="n">
-        <v>45.78</v>
+        <v>70.53</v>
       </c>
       <c r="D603" t="n">
-        <v>110.93</v>
+        <v>99.34999999999999</v>
       </c>
       <c r="E603" t="n">
-        <v>142.31</v>
+        <v>40.86</v>
       </c>
       <c r="F603" t="n">
-        <v>4.87571</v>
+        <v>3.37612</v>
       </c>
     </row>
     <row r="604">
       <c r="A604" t="inlineStr">
         <is>
-          <t>ADI</t>
+          <t>KRMN</t>
         </is>
       </c>
       <c r="B604" t="inlineStr">
@@ -14913,22 +14913,22 @@
         </is>
       </c>
       <c r="C604" t="n">
-        <v>223.95</v>
+        <v>45.78</v>
       </c>
       <c r="D604" t="n">
-        <v>318.7</v>
+        <v>110.93</v>
       </c>
       <c r="E604" t="n">
-        <v>42.31</v>
+        <v>142.31</v>
       </c>
       <c r="F604" t="n">
-        <v>6.15998</v>
+        <v>4.87571</v>
       </c>
     </row>
     <row r="605">
       <c r="A605" t="inlineStr">
         <is>
-          <t>TEVA</t>
+          <t>ADI</t>
         </is>
       </c>
       <c r="B605" t="inlineStr">
@@ -14937,22 +14937,22 @@
         </is>
       </c>
       <c r="C605" t="n">
-        <v>16.37</v>
+        <v>223.95</v>
       </c>
       <c r="D605" t="n">
-        <v>33.07</v>
+        <v>318.7</v>
       </c>
       <c r="E605" t="n">
-        <v>102.02</v>
+        <v>42.31</v>
       </c>
       <c r="F605" t="n">
-        <v>0.43058</v>
+        <v>6.15998</v>
       </c>
     </row>
     <row r="606">
       <c r="A606" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>BIO-B</t>
         </is>
       </c>
       <c r="B606" t="inlineStr">
@@ -14961,22 +14961,22 @@
         </is>
       </c>
       <c r="C606" t="n">
-        <v>285.13</v>
+        <v>247.05</v>
       </c>
       <c r="D606" t="n">
-        <v>352.1</v>
+        <v>312.75</v>
       </c>
       <c r="E606" t="n">
-        <v>23.49</v>
+        <v>26.59</v>
       </c>
       <c r="F606" t="n">
-        <v>2.00138</v>
+        <v>0.4732</v>
       </c>
     </row>
     <row r="607">
       <c r="A607" t="inlineStr">
         <is>
-          <t>FTAI</t>
+          <t>TEVA</t>
         </is>
       </c>
       <c r="B607" t="inlineStr">
@@ -14985,22 +14985,22 @@
         </is>
       </c>
       <c r="C607" t="n">
-        <v>136.06</v>
+        <v>16.37</v>
       </c>
       <c r="D607" t="n">
-        <v>276.01</v>
+        <v>33.07</v>
       </c>
       <c r="E607" t="n">
-        <v>102.86</v>
+        <v>102.02</v>
       </c>
       <c r="F607" t="n">
-        <v>11.21528</v>
+        <v>0.43058</v>
       </c>
     </row>
     <row r="608">
       <c r="A608" t="inlineStr">
         <is>
-          <t>BNS</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B608" t="inlineStr">
@@ -15009,22 +15009,22 @@
         </is>
       </c>
       <c r="C608" t="n">
-        <v>56</v>
+        <v>285.13</v>
       </c>
       <c r="D608" t="n">
-        <v>76.42</v>
+        <v>352.1</v>
       </c>
       <c r="E608" t="n">
-        <v>36.46</v>
+        <v>23.49</v>
       </c>
       <c r="F608" t="n">
-        <v>0.83523</v>
+        <v>2.00138</v>
       </c>
     </row>
     <row r="609">
       <c r="A609" t="inlineStr">
         <is>
-          <t>MLI</t>
+          <t>BNS</t>
         </is>
       </c>
       <c r="B609" t="inlineStr">
@@ -15033,22 +15033,22 @@
         </is>
       </c>
       <c r="C609" t="n">
-        <v>89.08</v>
+        <v>56</v>
       </c>
       <c r="D609" t="n">
-        <v>137.38</v>
+        <v>76.42</v>
       </c>
       <c r="E609" t="n">
-        <v>54.22</v>
+        <v>36.46</v>
       </c>
       <c r="F609" t="n">
-        <v>3.23044</v>
+        <v>0.83523</v>
       </c>
     </row>
     <row r="610">
       <c r="A610" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>TIGO</t>
         </is>
       </c>
       <c r="B610" t="inlineStr">
@@ -15057,22 +15057,22 @@
         </is>
       </c>
       <c r="C610" t="n">
-        <v>9.31</v>
+        <v>42.05</v>
       </c>
       <c r="D610" t="n">
-        <v>12.81</v>
+        <v>62.22</v>
       </c>
       <c r="E610" t="n">
-        <v>37.59</v>
+        <v>47.97</v>
       </c>
       <c r="F610" t="n">
-        <v>0.26373</v>
+        <v>1.76795</v>
       </c>
     </row>
     <row r="611">
       <c r="A611" t="inlineStr">
         <is>
-          <t>SLF</t>
+          <t>MLI</t>
         </is>
       </c>
       <c r="B611" t="inlineStr">
@@ -15081,22 +15081,22 @@
         </is>
       </c>
       <c r="C611" t="n">
-        <v>56.54</v>
+        <v>89.08</v>
       </c>
       <c r="D611" t="n">
-        <v>63.79</v>
+        <v>137.38</v>
       </c>
       <c r="E611" t="n">
-        <v>12.82</v>
+        <v>54.22</v>
       </c>
       <c r="F611" t="n">
-        <v>0.28712</v>
+        <v>3.23044</v>
       </c>
     </row>
     <row r="612">
       <c r="A612" t="inlineStr">
         <is>
-          <t>GH</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B612" t="inlineStr">
@@ -15105,22 +15105,22 @@
         </is>
       </c>
       <c r="C612" t="n">
-        <v>54.23</v>
+        <v>9.31</v>
       </c>
       <c r="D612" t="n">
-        <v>110.48</v>
+        <v>12.81</v>
       </c>
       <c r="E612" t="n">
-        <v>103.72</v>
+        <v>37.59</v>
       </c>
       <c r="F612" t="n">
-        <v>0.8918199999999999</v>
+        <v>0.26373</v>
       </c>
     </row>
     <row r="613">
       <c r="A613" t="inlineStr">
         <is>
-          <t>BBIO</t>
+          <t>SLF</t>
         </is>
       </c>
       <c r="B613" t="inlineStr">
@@ -15129,22 +15129,22 @@
         </is>
       </c>
       <c r="C613" t="n">
-        <v>46.58</v>
+        <v>56.54</v>
       </c>
       <c r="D613" t="n">
-        <v>79.09999999999999</v>
+        <v>63.79</v>
       </c>
       <c r="E613" t="n">
-        <v>69.81999999999999</v>
+        <v>12.82</v>
       </c>
       <c r="F613" t="n">
-        <v>0.51568</v>
+        <v>0.28712</v>
       </c>
     </row>
     <row r="614">
       <c r="A614" t="inlineStr">
         <is>
-          <t>BE</t>
+          <t>GH</t>
         </is>
       </c>
       <c r="B614" t="inlineStr">
@@ -15153,22 +15153,22 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>36.8</v>
+        <v>54.23</v>
       </c>
       <c r="D614" t="n">
-        <v>156.51</v>
+        <v>110.48</v>
       </c>
       <c r="E614" t="n">
-        <v>325.3</v>
+        <v>103.72</v>
       </c>
       <c r="F614" t="n">
-        <v>8.80753</v>
+        <v>0.8918199999999999</v>
       </c>
     </row>
     <row r="615">
       <c r="A615" t="inlineStr">
         <is>
-          <t>ARWR</t>
+          <t>BBIO</t>
         </is>
       </c>
       <c r="B615" t="inlineStr">
@@ -15177,22 +15177,22 @@
         </is>
       </c>
       <c r="C615" t="n">
-        <v>16.42</v>
+        <v>46.58</v>
       </c>
       <c r="D615" t="n">
-        <v>69.12</v>
+        <v>79.09999999999999</v>
       </c>
       <c r="E615" t="n">
-        <v>320.95</v>
+        <v>69.81999999999999</v>
       </c>
       <c r="F615" t="n">
-        <v>0.34305</v>
+        <v>0.51568</v>
       </c>
     </row>
     <row r="616">
       <c r="A616" t="inlineStr">
         <is>
-          <t>EDU</t>
+          <t>BE</t>
         </is>
       </c>
       <c r="B616" t="inlineStr">
@@ -15201,22 +15201,22 @@
         </is>
       </c>
       <c r="C616" t="n">
-        <v>45.58</v>
+        <v>36.8</v>
       </c>
       <c r="D616" t="n">
-        <v>59.46</v>
+        <v>156.51</v>
       </c>
       <c r="E616" t="n">
-        <v>30.45</v>
+        <v>325.3</v>
       </c>
       <c r="F616" t="n">
-        <v>0.47873</v>
+        <v>8.80753</v>
       </c>
     </row>
     <row r="617">
       <c r="A617" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>ARWR</t>
         </is>
       </c>
       <c r="B617" t="inlineStr">
@@ -15225,22 +15225,22 @@
         </is>
       </c>
       <c r="C617" t="n">
-        <v>19.95</v>
+        <v>16.42</v>
       </c>
       <c r="D617" t="n">
-        <v>48.66</v>
+        <v>69.12</v>
       </c>
       <c r="E617" t="n">
-        <v>143.91</v>
+        <v>320.95</v>
       </c>
       <c r="F617" t="n">
-        <v>0.39579</v>
+        <v>0.34305</v>
       </c>
     </row>
     <row r="618">
       <c r="A618" t="inlineStr">
         <is>
-          <t>FNV</t>
+          <t>EDU</t>
         </is>
       </c>
       <c r="B618" t="inlineStr">
@@ -15249,22 +15249,22 @@
         </is>
       </c>
       <c r="C618" t="n">
-        <v>171.59</v>
+        <v>45.58</v>
       </c>
       <c r="D618" t="n">
-        <v>261.77</v>
+        <v>59.46</v>
       </c>
       <c r="E618" t="n">
-        <v>52.56</v>
+        <v>30.45</v>
       </c>
       <c r="F618" t="n">
-        <v>9.51144</v>
+        <v>0.47873</v>
       </c>
     </row>
     <row r="619">
       <c r="A619" t="inlineStr">
         <is>
-          <t>VIK</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B619" t="inlineStr">
@@ -15273,22 +15273,22 @@
         </is>
       </c>
       <c r="C619" t="n">
-        <v>56.58</v>
+        <v>19.95</v>
       </c>
       <c r="D619" t="n">
-        <v>74.29000000000001</v>
+        <v>48.66</v>
       </c>
       <c r="E619" t="n">
-        <v>31.3</v>
+        <v>143.91</v>
       </c>
       <c r="F619" t="n">
-        <v>0.12575</v>
+        <v>0.39579</v>
       </c>
     </row>
     <row r="620">
       <c r="A620" t="inlineStr">
         <is>
-          <t>SPG</t>
+          <t>FNV</t>
         </is>
       </c>
       <c r="B620" t="inlineStr">
@@ -15297,64 +15297,64 @@
         </is>
       </c>
       <c r="C620" t="n">
-        <v>164.93</v>
+        <v>171.59</v>
       </c>
       <c r="D620" t="n">
-        <v>189.8</v>
+        <v>261.77</v>
       </c>
       <c r="E620" t="n">
-        <v>15.08</v>
+        <v>52.56</v>
       </c>
       <c r="F620" t="n">
-        <v>0.43519</v>
+        <v>9.51144</v>
       </c>
     </row>
     <row r="621">
       <c r="A621" t="inlineStr">
         <is>
-          <t>BIO-B</t>
+          <t>VIK</t>
         </is>
       </c>
       <c r="B621" t="inlineStr">
         <is>
-          <t>2025-08-07</t>
+          <t>2025-08-08</t>
         </is>
       </c>
       <c r="C621" t="n">
-        <v>247.05</v>
+        <v>56.58</v>
       </c>
       <c r="D621" t="n">
-        <v>312.75</v>
+        <v>74.29000000000001</v>
       </c>
       <c r="E621" t="n">
-        <v>26.59</v>
+        <v>31.3</v>
       </c>
       <c r="F621" t="n">
-        <v>0.52301</v>
+        <v>0.12575</v>
       </c>
     </row>
     <row r="622">
       <c r="A622" t="inlineStr">
         <is>
-          <t>MOG-B</t>
+          <t>SPG</t>
         </is>
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>2025-08-07</t>
+          <t>2025-08-08</t>
         </is>
       </c>
       <c r="C622" t="n">
-        <v>194.99</v>
+        <v>164.93</v>
       </c>
       <c r="D622" t="n">
-        <v>295</v>
+        <v>189.8</v>
       </c>
       <c r="E622" t="n">
-        <v>51.29</v>
+        <v>15.08</v>
       </c>
       <c r="F622" t="n">
-        <v>7.73238</v>
+        <v>0.43519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>